<commit_message>
Updates,Erros de Classificação e Treinamento completo no Excel
</commit_message>
<xml_diff>
--- a/@oatila1.xlsx
+++ b/@oatila1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/giovanniar_al_insper_edu_br/Documents/Desktop/Insper/2°Semestre DP/CDados/CD2020-Projeto1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - Insper - Institudo de Ensino e Pesquisa\Desktop\Insper\2°Semestre DP\CDados\CD2020-Projeto1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="490" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B3B8C464-79AE-497E-8C90-EC5430B25CC9}"/>
+  <xr:revisionPtr revIDLastSave="888" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E2D1907B-C8EE-4769-B6E5-2DA950C6CC19}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="713">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2390,7 +2390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2400,6 +2400,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2740,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="J290" sqref="J290"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="A200" sqref="A200:C301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4269,1065 +4272,1657 @@
       <c r="A139" t="s">
         <v>138</v>
       </c>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
+      <c r="B139" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="B140" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="B141" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
+      <c r="B142" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="B143" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
+      <c r="B144" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
+      <c r="B145" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
+      <c r="B146" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C146" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
+      <c r="B147" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C147" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
+      <c r="B148" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C148" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="B149" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
+      <c r="B150" s="5" t="s">
+        <v>708</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
+      <c r="B151" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
+      <c r="B152" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
+      <c r="B153" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
+      <c r="B154" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
+      <c r="B155" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
+      <c r="B156" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
+      <c r="B157" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="B158" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
+      <c r="B159" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
+      <c r="B160" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
+      <c r="B161" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
+      <c r="B162" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
+      <c r="B163" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>163</v>
       </c>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
+      <c r="B164" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>164</v>
       </c>
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
+      <c r="B165" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C165" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>165</v>
       </c>
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
+      <c r="B166" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C166" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
+      <c r="B167" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C167" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
+      <c r="B168" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C168" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
+      <c r="B169" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C169" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
+      <c r="B170" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C170" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
+      <c r="B171" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C171" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+      <c r="B172" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C172" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+      <c r="B173" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C173" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
+      <c r="B174" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
+      <c r="B175" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C175" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
+      <c r="B176" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C176" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
+      <c r="B177" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C177" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
+      <c r="B178" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C178" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
+      <c r="B179" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C179" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
+      <c r="B180" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C180" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>180</v>
       </c>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
+      <c r="B181" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
+      <c r="B182" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C182" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>182</v>
       </c>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
+      <c r="B183" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>183</v>
       </c>
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
+      <c r="B184" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>184</v>
       </c>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
+      <c r="B185" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C185" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>185</v>
       </c>
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
+      <c r="B186" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C186" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
+      <c r="B187" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C187" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>187</v>
       </c>
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
+      <c r="B188" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C188" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
+      <c r="B189" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C189" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
+      <c r="B190" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
+      <c r="B191" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+      <c r="B192" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="B193" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
+      <c r="B194" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C194" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
+      <c r="B195" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
+      <c r="B196" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
+      <c r="B197" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C197" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
+      <c r="B198" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C198" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-      <c r="B199" s="2"/>
-      <c r="C199" s="2"/>
+      <c r="B199" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C199" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
+      <c r="B200" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C200" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
+      <c r="B201" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C201" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-      <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
+      <c r="B202" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
+      <c r="B203" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C203" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
+      <c r="B204" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-      <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
+      <c r="B205" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C205" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>205</v>
       </c>
       <c r="B206" s="2"/>
-      <c r="C206" s="2"/>
+      <c r="C206" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
+      <c r="B207" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C207" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-      <c r="B208" s="2"/>
-      <c r="C208" s="2"/>
+      <c r="B208" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-      <c r="B209" s="2"/>
-      <c r="C209" s="2"/>
+      <c r="B209" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-      <c r="B210" s="2"/>
-      <c r="C210" s="2"/>
+      <c r="B210" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
+      <c r="B211" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C211" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
+      <c r="B212" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
+      <c r="B213" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
+      <c r="B214" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C214" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
+      <c r="B215" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
+      <c r="B216" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
+      <c r="B217" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C217" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>217</v>
       </c>
-      <c r="B218" s="2"/>
-      <c r="C218" s="2"/>
+      <c r="B218" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C218" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>218</v>
       </c>
-      <c r="B219" s="2"/>
-      <c r="C219" s="2"/>
+      <c r="B219" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C219" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>219</v>
       </c>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
+      <c r="B220" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
+      <c r="B221" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C221" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
+      <c r="B222" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>222</v>
       </c>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
+      <c r="B223" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C223" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
+      <c r="B224" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
+      <c r="B225" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C225" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
+      <c r="B226" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
+      <c r="B227" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
+      <c r="B228" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
+      <c r="B229" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-      <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
+      <c r="B230" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-      <c r="B231" s="2"/>
-      <c r="C231" s="2"/>
+      <c r="B231" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
+      <c r="B232" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
+      <c r="B233" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
+      <c r="B234" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-      <c r="B235" s="2"/>
-      <c r="C235" s="2"/>
+      <c r="B235" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C235" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-      <c r="B236" s="2"/>
-      <c r="C236" s="2"/>
+      <c r="B236" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-      <c r="B237" s="2"/>
-      <c r="C237" s="2"/>
+      <c r="B237" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C237" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
+      <c r="B238" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C238" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-      <c r="B239" s="2"/>
-      <c r="C239" s="2"/>
+      <c r="B239" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>239</v>
       </c>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
+      <c r="B240" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>240</v>
       </c>
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
+      <c r="B241" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>241</v>
       </c>
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
+      <c r="B242" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>242</v>
       </c>
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
+      <c r="B243" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>243</v>
       </c>
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
+      <c r="B244" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>244</v>
       </c>
       <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
+      <c r="C245" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>245</v>
       </c>
-      <c r="B246" s="2"/>
-      <c r="C246" s="2"/>
+      <c r="B246" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>246</v>
       </c>
-      <c r="B247" s="2"/>
-      <c r="C247" s="2"/>
+      <c r="B247" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>247</v>
       </c>
-      <c r="B248" s="2"/>
-      <c r="C248" s="2"/>
+      <c r="B248" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>248</v>
       </c>
-      <c r="B249" s="2"/>
-      <c r="C249" s="2"/>
+      <c r="B249" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>249</v>
       </c>
-      <c r="B250" s="2"/>
-      <c r="C250" s="2"/>
+      <c r="B250" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>250</v>
       </c>
-      <c r="B251" s="2"/>
-      <c r="C251" s="2"/>
+      <c r="B251" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>251</v>
       </c>
-      <c r="B252" s="2"/>
-      <c r="C252" s="2"/>
+      <c r="B252" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>252</v>
       </c>
-      <c r="B253" s="2"/>
-      <c r="C253" s="2"/>
+      <c r="B253" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>253</v>
       </c>
-      <c r="B254" s="2"/>
-      <c r="C254" s="2"/>
+      <c r="B254" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>254</v>
       </c>
       <c r="B255" s="2"/>
-      <c r="C255" s="2"/>
+      <c r="C255" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
-      <c r="B256" s="2"/>
-      <c r="C256" s="2"/>
+      <c r="B256" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>256</v>
       </c>
-      <c r="B257" s="2"/>
-      <c r="C257" s="2"/>
+      <c r="B257" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>257</v>
       </c>
-      <c r="B258" s="2"/>
-      <c r="C258" s="2"/>
+      <c r="B258" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C258" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>258</v>
       </c>
       <c r="B259" s="2"/>
-      <c r="C259" s="2"/>
+      <c r="C259" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>259</v>
       </c>
-      <c r="B260" s="2"/>
-      <c r="C260" s="2"/>
+      <c r="B260" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C260" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>260</v>
       </c>
-      <c r="B261" s="2"/>
-      <c r="C261" s="2"/>
+      <c r="B261" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C261" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>261</v>
       </c>
-      <c r="B262" s="2"/>
-      <c r="C262" s="2"/>
+      <c r="B262" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C262" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>262</v>
       </c>
-      <c r="B263" s="2"/>
-      <c r="C263" s="2"/>
+      <c r="B263" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C263" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>263</v>
       </c>
-      <c r="B264" s="2"/>
-      <c r="C264" s="2"/>
+      <c r="B264" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C264" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>264</v>
       </c>
-      <c r="B265" s="2"/>
-      <c r="C265" s="2"/>
+      <c r="B265" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C265" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>265</v>
       </c>
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
+      <c r="B266" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C266" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>266</v>
       </c>
       <c r="B267" s="2"/>
-      <c r="C267" s="2"/>
+      <c r="C267" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>267</v>
       </c>
-      <c r="B268" s="2"/>
-      <c r="C268" s="2"/>
+      <c r="B268" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C268" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>268</v>
       </c>
       <c r="B269" s="2"/>
-      <c r="C269" s="2"/>
+      <c r="C269" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>269</v>
       </c>
       <c r="B270" s="2"/>
-      <c r="C270" s="2"/>
+      <c r="C270" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>270</v>
       </c>
-      <c r="B271" s="2"/>
-      <c r="C271" s="2"/>
+      <c r="B271" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C271" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>271</v>
       </c>
       <c r="B272" s="2"/>
-      <c r="C272" s="2"/>
+      <c r="C272" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-      <c r="B273" s="2"/>
-      <c r="C273" s="2"/>
+      <c r="B273" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-      <c r="B274" s="2"/>
-      <c r="C274" s="2"/>
+      <c r="B274" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-      <c r="B275" s="2"/>
-      <c r="C275" s="2"/>
+      <c r="B275" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-      <c r="B276" s="2"/>
-      <c r="C276" s="2"/>
+      <c r="B276" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-      <c r="B277" s="2"/>
-      <c r="C277" s="2"/>
+      <c r="B277" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-      <c r="B278" s="2"/>
-      <c r="C278" s="2"/>
+      <c r="B278" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-      <c r="B279" s="2"/>
-      <c r="C279" s="2"/>
+      <c r="B279" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-      <c r="B280" s="2"/>
-      <c r="C280" s="2"/>
+      <c r="B280" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C280" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-      <c r="B281" s="2"/>
-      <c r="C281" s="2"/>
+      <c r="B281" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-      <c r="B282" s="2"/>
-      <c r="C282" s="2"/>
+      <c r="B282" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-      <c r="B283" s="2"/>
-      <c r="C283" s="2"/>
+      <c r="B283" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-      <c r="B284" s="2"/>
-      <c r="C284" s="2"/>
+      <c r="B284" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-      <c r="B285" s="2"/>
-      <c r="C285" s="2"/>
+      <c r="B285" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-      <c r="B286" s="2"/>
-      <c r="C286" s="2"/>
+      <c r="B286" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-      <c r="B287" s="2"/>
-      <c r="C287" s="2"/>
+      <c r="B287" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C287" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-      <c r="B288" s="2"/>
-      <c r="C288" s="2"/>
+      <c r="B288" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-      <c r="B289" s="2"/>
-      <c r="C289" s="2"/>
+      <c r="B289" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C289" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-      <c r="B290" s="2"/>
-      <c r="C290" s="2"/>
+      <c r="B290" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C290" s="2" t="s">
+        <v>703</v>
+      </c>
       <c r="F290" s="3"/>
       <c r="J290" s="3"/>
     </row>
@@ -5335,79 +5930,123 @@
       <c r="A291" t="s">
         <v>290</v>
       </c>
-      <c r="B291" s="2"/>
-      <c r="C291" s="2"/>
+      <c r="B291" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C291" s="2" t="s">
+        <v>704</v>
+      </c>
       <c r="F291" s="3"/>
     </row>
     <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-      <c r="B292" s="2"/>
-      <c r="C292" s="2"/>
+      <c r="B292" s="2" t="s">
+        <v>712</v>
+      </c>
+      <c r="C292" s="2" t="s">
+        <v>704</v>
+      </c>
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-      <c r="B293" s="2"/>
-      <c r="C293" s="2"/>
+      <c r="B293" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C293" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-      <c r="B294" s="2"/>
-      <c r="C294" s="2"/>
+      <c r="B294" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-      <c r="B295" s="2"/>
-      <c r="C295" s="2"/>
+      <c r="B295" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C295" s="2" t="s">
+        <v>706</v>
+      </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-      <c r="B296" s="2"/>
-      <c r="C296" s="2"/>
+      <c r="B296" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="C296" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-      <c r="B297" s="2"/>
-      <c r="C297" s="2"/>
+      <c r="B297" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-      <c r="B298" s="2"/>
-      <c r="C298" s="2"/>
+      <c r="B298" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-      <c r="B299" s="2"/>
-      <c r="C299" s="2"/>
+      <c r="B299" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="C299" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-      <c r="B300" s="2"/>
-      <c r="C300" s="2"/>
+      <c r="B300" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C300" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>300</v>
       </c>
-      <c r="B301" s="2"/>
-      <c r="C301" s="2"/>
+      <c r="B301" s="5" t="s">
+        <v>705</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>703</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5419,8 +6058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="B384" sqref="B384"/>
+    <sheetView topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="A401" sqref="A401:C406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Excel a finalizar; Notebook pronto
</commit_message>
<xml_diff>
--- a/@oatila1.xlsx
+++ b/@oatila1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive - Insper - Institudo de Ensino e Pesquisa\Desktop\Insper\2°Semestre DP\CDados\CD2020-Projeto1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/giovanniar_al_insper_edu_br/Documents/Desktop/Insper/2°Semestre DP/CDados/CD2020-Projeto1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="888" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E2D1907B-C8EE-4769-B6E5-2DA950C6CC19}"/>
+  <xr:revisionPtr revIDLastSave="930" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B865E6B9-9D34-43B6-B905-27DD73CBA48D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="713">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2743,7 +2743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+    <sheetView topLeftCell="A198" workbookViewId="0">
       <selection activeCell="A200" sqref="A200:C301"/>
     </sheetView>
   </sheetViews>
@@ -6058,8 +6058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B400"/>
   <sheetViews>
-    <sheetView topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="A401" sqref="A401:C406"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6504,208 +6504,316 @@
       <c r="A55" t="s">
         <v>355</v>
       </c>
+      <c r="B55" s="4" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>356</v>
       </c>
+      <c r="B56" s="4" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>357</v>
       </c>
+      <c r="B57" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>358</v>
       </c>
+      <c r="B58" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>359</v>
       </c>
+      <c r="B59" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>360</v>
       </c>
+      <c r="B60" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>361</v>
       </c>
+      <c r="B61" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>362</v>
       </c>
+      <c r="B62" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>363</v>
       </c>
+      <c r="B63" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>396</v>
       </c>

</xml_diff>

<commit_message>
Versão 4- Excel 100% Notebook com novos erros- Trabalhando nisso
</commit_message>
<xml_diff>
--- a/@oatila1.xlsx
+++ b/@oatila1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alinsperedu-my.sharepoint.com/personal/giovanniar_al_insper_edu_br/Documents/Desktop/Insper/2°Semestre DP/CDados/CD2020-Projeto1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="930" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{B865E6B9-9D34-43B6-B905-27DD73CBA48D}"/>
+  <xr:revisionPtr revIDLastSave="1273" documentId="11_57AEF0097B73D09A7ED7105EC318E145E12F6EDF" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8FD1ED49-6488-4386-940C-66FF4C7EF7C1}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1879" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1692" uniqueCount="713">
   <si>
     <t>Treinamento</t>
   </si>
@@ -2743,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J301"/>
   <sheetViews>
-    <sheetView topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200:C301"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6056,10 +6056,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B400"/>
+  <dimension ref="A1:J400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6068,7 +6068,7 @@
     <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>301</v>
       </c>
@@ -6076,7 +6076,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>302</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>303</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>304</v>
       </c>
@@ -6100,7 +6100,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>305</v>
       </c>
@@ -6108,7 +6108,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>307</v>
       </c>
@@ -6124,23 +6124,24 @@
         <v>708</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>308</v>
       </c>
       <c r="B8" t="s">
         <v>705</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>309</v>
       </c>
-      <c r="B9" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>310</v>
       </c>
@@ -6148,7 +6149,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>311</v>
       </c>
@@ -6156,7 +6157,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>312</v>
       </c>
@@ -6164,7 +6165,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>313</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>314</v>
       </c>
@@ -6180,7 +6181,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>315</v>
       </c>
@@ -6188,7 +6189,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -6792,1388 +6793,2219 @@
       <c r="A91" t="s">
         <v>391</v>
       </c>
+      <c r="B91" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>392</v>
       </c>
+      <c r="B92" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>393</v>
       </c>
+      <c r="B93" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>394</v>
       </c>
+      <c r="B94" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>395</v>
       </c>
+      <c r="B95" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B118" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B119" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B165" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B166" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B167" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B168" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B169" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B170" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B173" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B174" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B175" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B177" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B178" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B179" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B180" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B181" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B182" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B183" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B184" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B186" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B187" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B188" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B189" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B190" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B191" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B192" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B193" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B194" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B195" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B196" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B197" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B198" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B199" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B200" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B201" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B202" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B203" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B204" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B205" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B206" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B207" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B208" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B209" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B210" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B211" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B212" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B213" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B214" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B215" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B216" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B217" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B218" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B219" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B220" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B221" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B222" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B223" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B224" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B225" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B226" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B227" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B228" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B229" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B230" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B231" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B232" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B233" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B234" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B235" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B236" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B237" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B238" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B239" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B240" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B241" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B242" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B243" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B244" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B245" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B246" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B247" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B248" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B249" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B250" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B251" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B252" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B253" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B254" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B255" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B256" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B257" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B258" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B259" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B260" s="3" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B261" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B262" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B263" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B264" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B265" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B266" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B267" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B268" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B269" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B270" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B271" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B272" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B273" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B274" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>575</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B275" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B276" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>577</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B277" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>578</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B278" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B279" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>580</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B280" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B281" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B282" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>583</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B283" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B284" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>585</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B285" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>586</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B286" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B287" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B288" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>589</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B289" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B290" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>591</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B291" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>592</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B292" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>593</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B293" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B294" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>595</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B295" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>596</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B296" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>597</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B297" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>598</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B298" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B299" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>600</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B300" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>601</v>
       </c>
-    </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B301" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>602</v>
       </c>
-    </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B302" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>603</v>
       </c>
-    </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B303" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>604</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B304" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>605</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B305" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>606</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B306" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>607</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B307" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B308" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>609</v>
       </c>
-    </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B309" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>610</v>
       </c>
-    </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B310" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>611</v>
       </c>
-    </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B311" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>612</v>
       </c>
-    </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B312" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>613</v>
       </c>
-    </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B313" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>614</v>
       </c>
-    </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B314" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>615</v>
       </c>
-    </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B315" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B316" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>617</v>
       </c>
-    </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B317" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>618</v>
       </c>
-    </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B318" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>619</v>
       </c>
-    </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B319" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>620</v>
       </c>
-    </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B320" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>621</v>
       </c>
-    </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B321" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B322" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>623</v>
       </c>
-    </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B323" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>624</v>
       </c>
-    </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B324" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>625</v>
       </c>
-    </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B325" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>626</v>
       </c>
-    </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B326" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>627</v>
       </c>
-    </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B327" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>628</v>
       </c>
-    </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B328" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>629</v>
       </c>
-    </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B329" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>630</v>
       </c>
-    </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B330" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>631</v>
       </c>
-    </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B331" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>632</v>
       </c>
-    </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B332" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>633</v>
       </c>
-    </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B333" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>634</v>
       </c>
-    </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B334" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>635</v>
       </c>
-    </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B335" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>636</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B336" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>637</v>
       </c>
-    </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B337" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>638</v>
       </c>
-    </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B338" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>639</v>
       </c>
-    </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B339" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>640</v>
       </c>
-    </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B340" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>641</v>
       </c>
-    </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B341" s="3" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>642</v>
       </c>
-    </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B342" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>643</v>
       </c>
-    </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B343" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>644</v>
       </c>
-    </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B344" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>645</v>
       </c>
-    </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B345" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B346" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>647</v>
       </c>
-    </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B347" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B348" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>649</v>
       </c>
-    </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B349" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>650</v>
       </c>
-    </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B350" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>651</v>
       </c>
-    </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B351" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B352" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>653</v>
       </c>
-    </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B353" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>654</v>
       </c>
-    </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B354" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>655</v>
       </c>
-    </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B355" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B356" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B357" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>658</v>
       </c>
-    </row>
-    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B358" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>659</v>
       </c>
-    </row>
-    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B359" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>660</v>
       </c>
-    </row>
-    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B360" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>661</v>
       </c>
-    </row>
-    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B361" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>662</v>
       </c>
-    </row>
-    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B362" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>663</v>
       </c>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B363" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B364" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B365" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>666</v>
       </c>
-    </row>
-    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B366" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>667</v>
       </c>
-    </row>
-    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B367" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>668</v>
       </c>
@@ -8182,66 +9014,105 @@
       <c r="A369" t="s">
         <v>669</v>
       </c>
+      <c r="B369" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>670</v>
       </c>
+      <c r="B370" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>671</v>
       </c>
+      <c r="B371" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>672</v>
       </c>
+      <c r="B372" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>673</v>
       </c>
+      <c r="B373" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>674</v>
       </c>
+      <c r="B374" t="s">
+        <v>708</v>
+      </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>675</v>
       </c>
+      <c r="B375" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>676</v>
       </c>
+      <c r="B376" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>677</v>
       </c>
+      <c r="B377" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>678</v>
       </c>
+      <c r="B378" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>679</v>
       </c>
+      <c r="B379" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>680</v>
       </c>
+      <c r="B380" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>681</v>
       </c>
+      <c r="B381" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -8255,6 +9126,9 @@
       <c r="A383" t="s">
         <v>683</v>
       </c>
+      <c r="B383" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
@@ -8268,16 +9142,25 @@
       <c r="A385" t="s">
         <v>685</v>
       </c>
+      <c r="B385" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>686</v>
       </c>
+      <c r="B386" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>687</v>
       </c>
+      <c r="B387" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
@@ -8291,55 +9174,88 @@
       <c r="A389" t="s">
         <v>689</v>
       </c>
+      <c r="B389" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>690</v>
       </c>
+      <c r="B390" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>691</v>
       </c>
+      <c r="B391" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>692</v>
       </c>
+      <c r="B392" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>693</v>
       </c>
+      <c r="B393" t="s">
+        <v>709</v>
+      </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>694</v>
       </c>
+      <c r="B394" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>695</v>
       </c>
+      <c r="B395" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>696</v>
       </c>
+      <c r="B396" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>697</v>
       </c>
+      <c r="B397" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>698</v>
       </c>
+      <c r="B398" t="s">
+        <v>705</v>
+      </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>699</v>
+      </c>
+      <c r="B399" t="s">
+        <v>707</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>